<commit_message>
Added a few rooms to map
added tunnel and crystal cavern
</commit_message>
<xml_diff>
--- a/Project 14 Map.xlsx
+++ b/Project 14 Map.xlsx
@@ -19,12 +19,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Start: Grate in floor D,  Archway  N, Wooden Door  S, E</t>
   </si>
   <si>
     <t>Rising Room U, D, S</t>
+  </si>
+  <si>
+    <t>Low Winding Tunnel N, E</t>
+  </si>
+  <si>
+    <t>Crystal Cavern W, E, S, Crystal Shard(requires pickaxe), Unlit Lantern, Pickaxe,</t>
   </si>
 </sst>
 </file>
@@ -111,7 +117,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -132,11 +138,15 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -319,7 +329,7 @@
   <dimension ref="C1:D3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="71.7"/>
@@ -336,10 +346,15 @@
       <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="71.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Made Changes To Map
Added more rooms and started the walkthrough
</commit_message>
<xml_diff>
--- a/Project 14 Map.xlsx
+++ b/Project 14 Map.xlsx
@@ -5,32 +5,185 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="295" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="295" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Sheet5" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Sheet5" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Sheet4" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Start: Grate in floor D,  Archway  N, Wooden Door  S, E</t>
-  </si>
-  <si>
-    <t>Rising Room U, D, S</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
+  <si>
+    <t>Wizard's Wardrobe Door E, Wizard's Robe, Wizard's Hat</t>
+  </si>
+  <si>
+    <t>Wizard's Grotto Door W, Archway S Old Carved Staff (Broken)</t>
+  </si>
+  <si>
+    <t>Start: Grate in floor D,  Archway  N, Wooden Door  S, Iron Door E,</t>
+  </si>
+  <si>
+    <t>Warp Ring</t>
+  </si>
+  <si>
+    <t>Storeroom  N, Coal, Backpack, Glow Moss</t>
+  </si>
+  <si>
+    <t>Start by going S into the coal room.</t>
+  </si>
+  <si>
+    <t>Take the moss</t>
+  </si>
+  <si>
+    <t>Put the coal in the backpack</t>
+  </si>
+  <si>
+    <t>Take the coal backpack</t>
+  </si>
+  <si>
+    <t>Go N to start room</t>
+  </si>
+  <si>
+    <t>Go N to Wizard's Grotto</t>
+  </si>
+  <si>
+    <t>Take the staff and the spellbook</t>
+  </si>
+  <si>
+    <t>Go S to start room</t>
+  </si>
+  <si>
+    <t>Open the grate</t>
+  </si>
+  <si>
+    <t>Hop down (Coal weighs you down)</t>
+  </si>
+  <si>
+    <t>Go S to the winding tunnel</t>
+  </si>
+  <si>
+    <t>Go E to the crystal cavern</t>
+  </si>
+  <si>
+    <t>Inspect ground</t>
+  </si>
+  <si>
+    <t>Take the flint</t>
+  </si>
+  <si>
+    <t>Light lantern with flint</t>
+  </si>
+  <si>
+    <t>Go E to the crystal hall</t>
+  </si>
+  <si>
+    <t>Go E to the throne room</t>
+  </si>
+  <si>
+    <t>Inspect Throne</t>
+  </si>
+  <si>
+    <t>Take coal out of backpack</t>
+  </si>
+  <si>
+    <t>Drop coal</t>
+  </si>
+  <si>
+    <t>Take pickaxe and war hammer</t>
+  </si>
+  <si>
+    <t>Go W to the crystal hall</t>
+  </si>
+  <si>
+    <t>Go W to the crystal cavern</t>
+  </si>
+  <si>
+    <t>Break crystal with pickaxe</t>
+  </si>
+  <si>
+    <t>Take crystal shard</t>
+  </si>
+  <si>
+    <t>Go W to the low winding tunnel</t>
+  </si>
+  <si>
+    <t>Go N to the start room</t>
+  </si>
+  <si>
+    <t>Go N to the wizard's grotto</t>
+  </si>
+  <si>
+    <t>Go W to the wizard's wardrobe</t>
+  </si>
+  <si>
+    <t>Take the wizard's robes</t>
+  </si>
+  <si>
+    <t>Go E to the wizard's grotto</t>
+  </si>
+  <si>
+    <t>Go S to the start room</t>
+  </si>
+  <si>
+    <t>Equip Wizard's Robes and Hammer</t>
+  </si>
+  <si>
+    <t>Inspect spellbook</t>
+  </si>
+  <si>
+    <t>Speak chocolate spell</t>
+  </si>
+  <si>
+    <t>Break chocolate door with hammer</t>
+  </si>
+  <si>
+    <t>Take chocolate slab</t>
+  </si>
+  <si>
+    <t>Take warp ring</t>
+  </si>
+  <si>
+    <t>Use warp spell</t>
+  </si>
+  <si>
+    <t>Rising Room U, S</t>
   </si>
   <si>
     <t>Low Winding Tunnel N, E</t>
   </si>
   <si>
-    <t>Crystal Cavern W, E, S, Crystal Shard(requires pickaxe), Unlit Lantern, Pickaxe,</t>
+    <t>Crystal Cavern W, E, Crystal Shard(requires pickaxe), Unlit Lantern, Flint</t>
+  </si>
+  <si>
+    <t>Crystal Hall W, E</t>
+  </si>
+  <si>
+    <t>Dwarven Throne W, Pickaxe, War Hammer</t>
+  </si>
+  <si>
+    <t>Wizard's Grotto Door W, Old Carved Staff (Broken)</t>
+  </si>
+  <si>
+    <t>Start: Grate in floor D,  Archway  N, Wooden Door  S, Iron Door E</t>
+  </si>
+  <si>
+    <t>Flat Shovel</t>
+  </si>
+  <si>
+    <t>Water Room U, Stone/Dirt Wall S</t>
+  </si>
+  <si>
+    <t>Low Winding Tunnel N, S</t>
+  </si>
+  <si>
+    <t>Crystal Cavern W, E</t>
   </si>
 </sst>
 </file>
@@ -63,7 +216,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -78,8 +231,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00CC33"/>
-        <bgColor rgb="FF339966"/>
+        <fgColor rgb="FF33FF99"/>
+        <bgColor rgb="FF00FFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9999"/>
+        <bgColor rgb="FFFF8080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFCCFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -117,20 +282,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -138,15 +303,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -164,7 +325,7 @@
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00CC33"/>
+      <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -184,7 +345,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -198,11 +359,11 @@
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFFF9999"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF33FF99"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
@@ -227,20 +388,39 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="B1:D3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="72.55"/>
+  <sheetFormatPr defaultRowHeight="71.7"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="51.7755102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="12.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="2" width="12.9030612244898"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="71.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="3" customFormat="false" ht="71.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1" customFormat="false" ht="71.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="71.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="71.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C3" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -257,18 +437,213 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A39"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="71.7"/>
+  <sheetFormatPr defaultRowHeight="36.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="51.7755102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="12.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="2" width="155.489795918367"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="36.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -284,31 +659,40 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:D3"/>
+  <dimension ref="C1:F3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="71.7"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="51.7755102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="12.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="51.7755102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="2" width="12.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="71.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="2"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="71.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="3"/>
+      <c r="C2" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="71.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -326,34 +710,37 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C1:D3"/>
+  <dimension ref="B1:D3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="71.7"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="51.7755102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="12.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="2" width="12.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="71.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C1" s="5"/>
-      <c r="D1" s="2"/>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="71.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="7"/>
+      <c r="C2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="71.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -372,18 +759,42 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="C1:F3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="71.7"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="51.7755102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="12.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="51.7755102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="2" width="12.9030612244898"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="71.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="71.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C2" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="71.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>